<commit_message>
included addition/clarification from sir Dondon
</commit_message>
<xml_diff>
--- a/Zenkoku Hoshou Training Documentation.xlsx
+++ b/Zenkoku Hoshou Training Documentation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8295" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="19890" windowHeight="8295" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251">
   <si>
     <t>Training Item</t>
   </si>
@@ -651,7 +651,7 @@
     <t>PG</t>
   </si>
   <si>
-    <t>explained by person who requested</t>
+    <t>explained by person who investigated</t>
   </si>
   <si>
     <t>if person who requested is not present, somebody who has knowledge in the request will explain</t>
@@ -672,6 +672,12 @@
     <t>folder for deliverables</t>
   </si>
   <si>
+    <t>there are instances where one AWS member is 開発SE and another is PG</t>
+  </si>
+  <si>
+    <t>in an 案件, it is possible that AWS member is not included</t>
+  </si>
+  <si>
     <t>KAIHATSU PROPER</t>
   </si>
   <si>
@@ -712,8 +718,7 @@
   </si>
   <si>
     <t>UT Environments:
-Portal environment
-Test terminal for IE9 (remote access)</t>
+Dev environment via Test terminals</t>
   </si>
   <si>
     <t>Check in</t>
@@ -740,9 +745,17 @@
     <t>if there is no 設計SE, it is reviewed by 開発SE</t>
   </si>
   <si>
-    <t>IT Environments:
-IE9 (online)
-1号機 and 2号機 (batch job)</t>
+    <t xml:space="preserve">IT Environments:
+1号機 and 2号機 </t>
+  </si>
+  <si>
+    <t>For online test:
+access 1号機 or 2号機 through IE9</t>
+  </si>
+  <si>
+    <t>For batch:
+need to log-on to 1号機 or 2号機 PC, and
+execute single batch file. if need to execute multiple batch files, use JP1 application</t>
   </si>
   <si>
     <t>Management</t>
@@ -790,9 +803,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -825,10 +838,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -841,14 +879,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -863,72 +915,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -954,8 +944,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -994,7 +1007,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,25 +1169,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,145 +1187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,10 +1320,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1320,7 +1331,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1370,24 +1381,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1402,12 +1395,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1425,134 +1438,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1587,6 +1600,30 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2278,113 +2315,113 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="37.2857142857143" style="50" customWidth="1"/>
-    <col min="2" max="2" width="19.4285714285714" style="50" customWidth="1"/>
-    <col min="3" max="3" width="14.5714285714286" style="50" customWidth="1"/>
-    <col min="4" max="4" width="15.5714285714286" style="50" customWidth="1"/>
-    <col min="5" max="5" width="26.4285714285714" style="50" customWidth="1"/>
-    <col min="6" max="16383" width="9.14285714285714" style="50"/>
+    <col min="1" max="1" width="37.2857142857143" style="58" customWidth="1"/>
+    <col min="2" max="2" width="19.4285714285714" style="58" customWidth="1"/>
+    <col min="3" max="3" width="14.5714285714286" style="58" customWidth="1"/>
+    <col min="4" max="4" width="15.5714285714286" style="58" customWidth="1"/>
+    <col min="5" max="5" width="26.4285714285714" style="58" customWidth="1"/>
+    <col min="6" max="16383" width="9.14285714285714" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="61">
         <v>43566</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="61">
         <v>43566</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="61">
         <v>43566</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="61">
         <v>43566</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="61">
         <v>43571</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="61">
         <v>43571</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="61">
         <v>43571</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="61">
         <v>43571</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="61">
         <v>43571</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="61">
         <v>43571</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="61">
         <v>43571</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="61">
         <v>43571</v>
       </c>
     </row>
@@ -2414,15 +2451,15 @@
   </cols>
   <sheetData>
     <row r="1" ht="47" customHeight="1" spans="1:5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="39"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
@@ -2440,7 +2477,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="55" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="8"/>
@@ -2451,7 +2488,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="55" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="8"/>
@@ -2461,7 +2498,7 @@
       <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="56" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2470,12 +2507,12 @@
       <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="57" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
@@ -2629,7 +2666,7 @@
   <sheetPr/>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2649,18 +2686,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="45"/>
+      <c r="D1" s="44" t="s">
         <v>47</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="47"/>
       <c r="I1"/>
       <c r="J1"/>
     </row>
@@ -2673,7 +2710,7 @@
         <v>49</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="48" t="s">
         <v>50</v>
       </c>
       <c r="I2"/>
@@ -2686,7 +2723,7 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="5"/>
-      <c r="G3" s="41"/>
+      <c r="G3" s="49"/>
       <c r="I3"/>
       <c r="J3"/>
     </row>
@@ -2697,7 +2734,7 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="41"/>
+      <c r="G4" s="49"/>
       <c r="I4"/>
       <c r="J4"/>
     </row>
@@ -2708,7 +2745,7 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="41"/>
+      <c r="G5" s="49"/>
       <c r="I5"/>
       <c r="J5"/>
     </row>
@@ -2719,7 +2756,7 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="50" t="s">
         <v>55</v>
       </c>
       <c r="I6"/>
@@ -2732,7 +2769,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="G7" s="41"/>
+      <c r="G7" s="49"/>
       <c r="I7"/>
       <c r="J7"/>
     </row>
@@ -2745,7 +2782,7 @@
       <c r="E8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="49"/>
       <c r="I8"/>
       <c r="J8"/>
     </row>
@@ -2758,7 +2795,7 @@
       <c r="E9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="51" t="s">
         <v>60</v>
       </c>
       <c r="I9"/>
@@ -2773,7 +2810,7 @@
       <c r="E10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="52" t="s">
         <v>63</v>
       </c>
       <c r="I10"/>
@@ -2784,7 +2821,7 @@
       <c r="B11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="45"/>
+      <c r="G11" s="53"/>
       <c r="I11"/>
       <c r="J11"/>
     </row>
@@ -2845,7 +2882,7 @@
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="54" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="5"/>
@@ -2924,7 +2961,7 @@
       <c r="D1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" ht="21" customHeight="1" spans="1:6">
@@ -2932,13 +2969,13 @@
         <v>80</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="37" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2947,54 +2984,54 @@
       <c r="B3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="38" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="39" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="4" ht="30" spans="1:6">
       <c r="A4" s="8"/>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="38" t="s">
         <v>89</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="39" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" ht="110" customHeight="1" spans="1:6">
       <c r="A5" s="8"/>
       <c r="B5" s="5"/>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="38" t="s">
         <v>92</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="39" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="8"/>
       <c r="B6" s="5"/>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="38" t="s">
         <v>95</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="39" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3003,13 +3040,13 @@
         <v>98</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="38" t="s">
         <v>99</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="39" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3018,13 +3055,13 @@
       <c r="B8" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="38" t="s">
         <v>103</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="39" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3033,13 +3070,13 @@
       <c r="B9" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="38" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="39" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3048,13 +3085,13 @@
       <c r="B10" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="38" t="s">
         <v>111</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="39" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3063,134 +3100,134 @@
       <c r="B11" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="38" t="s">
         <v>115</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="39" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" spans="4:6">
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="38" t="s">
         <v>118</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="39" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="13" spans="4:6">
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="38" t="s">
         <v>121</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="39" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="14" spans="4:6">
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="38" t="s">
         <v>124</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="39" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="15" spans="4:6">
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="38" t="s">
         <v>127</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="39" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" spans="4:6">
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="38" t="s">
         <v>130</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="39" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" spans="4:6">
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="38" t="s">
         <v>133</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="39" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="18" spans="4:6">
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="38" t="s">
         <v>136</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="39" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="19" spans="4:6">
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="38" t="s">
         <v>139</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="39" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="20" spans="4:6">
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="38" t="s">
         <v>142</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="39" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="21" spans="4:6">
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="38" t="s">
         <v>145</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="39" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="22" spans="4:6">
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="43" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3224,108 +3261,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="22"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="30" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="30" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="30"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="30" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="30"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="30"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="30" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="30"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="30"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="30" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="30" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="30" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="22" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="30" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="30"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="30"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="32"/>
+      <c r="B19" s="33" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3341,10 +3378,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3394,10 +3431,10 @@
         <v>171</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="8"/>
@@ -3412,8 +3449,8 @@
       <c r="H3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" ht="60" spans="1:8">
       <c r="A4" s="8"/>
@@ -3490,8 +3527,8 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="8"/>
@@ -3502,8 +3539,8 @@
         <v>190</v>
       </c>
       <c r="H10" s="5"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="8"/>
@@ -3516,8 +3553,8 @@
       <c r="E11" s="5"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="8"/>
@@ -3528,8 +3565,8 @@
       <c r="E12" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="8"/>
@@ -3540,16 +3577,16 @@
       <c r="E13" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="8"/>
       <c r="B14" s="5"/>
       <c r="D14" s="8"/>
       <c r="E14" s="5"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
@@ -3560,8 +3597,8 @@
         <v>198</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="8"/>
@@ -3572,8 +3609,8 @@
       <c r="E16" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="8"/>
@@ -3584,8 +3621,8 @@
       <c r="E17" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="8"/>
@@ -3596,8 +3633,8 @@
       <c r="E18" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" ht="45" spans="1:11">
       <c r="A19" s="11" t="s">
@@ -3608,8 +3645,8 @@
       <c r="E19" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="8"/>
@@ -3618,8 +3655,8 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="5"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" ht="30" spans="1:5">
       <c r="A21" s="8"/>
@@ -3632,8 +3669,8 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" ht="45" spans="1:5">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5" t="s">
         <v>209</v>
       </c>
       <c r="D22" s="8"/>
@@ -3641,26 +3678,34 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="4:5">
+    <row r="23" ht="45" spans="1:5">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13" t="s">
+        <v>211</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="4:5">
+    <row r="24" ht="45" spans="1:5">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15" t="s">
+        <v>212</v>
+      </c>
       <c r="D24" s="11" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="4:5">
       <c r="D25" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="4:5">
       <c r="D26" s="8"/>
       <c r="E26" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="4:5">
@@ -3669,7 +3714,7 @@
     </row>
     <row r="28" spans="4:5">
       <c r="D28" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -3679,26 +3724,26 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="4:5">
       <c r="D31" s="8"/>
       <c r="E31" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" ht="30" spans="4:5">
       <c r="D32" s="8"/>
       <c r="E32" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="4:5">
       <c r="D33" s="8"/>
       <c r="E33" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="4:5">
@@ -3707,20 +3752,20 @@
     </row>
     <row r="35" spans="4:5">
       <c r="D35" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="4:5">
       <c r="D36" s="8"/>
       <c r="E36" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="4:5">
       <c r="D37" s="8"/>
       <c r="E37" s="5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="4:5">
@@ -3729,26 +3774,26 @@
     </row>
     <row r="39" spans="4:5">
       <c r="D39" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="4:5">
       <c r="D40" s="8"/>
       <c r="E40" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="4:5">
       <c r="D41" s="8"/>
       <c r="E41" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" ht="60" spans="4:5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" ht="45" spans="4:5">
       <c r="D42" s="8"/>
       <c r="E42" s="5" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="4:5">
@@ -3757,14 +3802,14 @@
     </row>
     <row r="44" spans="4:5">
       <c r="D44" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="4:5">
       <c r="D45" s="8"/>
       <c r="E45" s="5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="4:5">
@@ -3773,20 +3818,20 @@
     </row>
     <row r="47" spans="4:5">
       <c r="D47" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="4:5">
       <c r="D48" s="8"/>
       <c r="E48" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" ht="30" spans="4:5">
       <c r="D49" s="8"/>
       <c r="E49" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="4:5">
@@ -3795,26 +3840,38 @@
     </row>
     <row r="51" spans="4:5">
       <c r="D51" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="4:5">
       <c r="D52" s="8"/>
       <c r="E52" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" ht="30" spans="4:5">
       <c r="D53" s="8"/>
       <c r="E53" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="54" ht="60" spans="4:5">
-      <c r="D54" s="6"/>
-      <c r="E54" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" ht="45" spans="4:5">
+      <c r="D54" s="8"/>
+      <c r="E54" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="55" ht="45" spans="4:5">
+      <c r="D55" s="16"/>
+      <c r="E55" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" ht="120" spans="4:5">
+      <c r="D56" s="18"/>
+      <c r="E56" s="19" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3855,15 +3912,15 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B1" s="3"/>
       <c r="D1" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E1" s="3"/>
       <c r="G1" s="2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -3873,26 +3930,26 @@
       </c>
       <c r="B2" s="5"/>
       <c r="D2" s="4" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E2" s="5"/>
       <c r="G2" s="4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H2" s="5"/>
     </row>
     <row r="3" ht="60" spans="1:8">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="5" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="4:5">
@@ -3901,7 +3958,7 @@
     </row>
     <row r="5" spans="4:8">
       <c r="D5" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E5" s="5"/>
       <c r="G5" s="9"/>
@@ -3910,7 +3967,7 @@
     <row r="6" spans="4:8">
       <c r="D6" s="8"/>
       <c r="E6" s="5" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -3918,7 +3975,7 @@
     <row r="7" ht="45" spans="4:5">
       <c r="D7" s="8"/>
       <c r="E7" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="4:5">
@@ -3927,14 +3984,14 @@
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="4" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>